<commit_message>
Fixed issues in code
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine11.xlsx
+++ b/bin/dataEngine/DataEngine11.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D14D4FC-6B86-4B15-A950-0F28831A985A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16665" windowHeight="6135"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Steps" sheetId="1" r:id="rId2"/>
     <sheet name="Settings" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -19,12 +20,11 @@
     <definedName name="Page_Name">Settings!$A$2:$A$10</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -183,13 +183,15 @@
   </si>
   <si>
     <t>Action Keywords</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,6 +255,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -300,7 +305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +338,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,6 +390,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,244 +582,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="39.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="10.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D11 F1:F11">
-      <formula1>Page_Name</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,8 +638,237 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D11 F1:F11" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>Page_Name</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -835,10 +877,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated mouseHover action keyword
</commit_message>
<xml_diff>
--- a/bin/dataEngine/DataEngine11.xlsx
+++ b/bin/dataEngine/DataEngine11.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EDDA8-4DB3-47AB-8A5E-1C79392D6862}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018DD7B6-C326-4BDD-BC11-3176712135C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Login in into Amazon</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>mouseHover</t>
+  </si>
+  <si>
+    <t>Login in and log out into Amazon</t>
+  </si>
+  <si>
+    <t>zeba</t>
   </si>
 </sst>
 </file>
@@ -597,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +622,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,10 +630,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,10 +655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -690,10 +693,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -710,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -758,10 +761,10 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -769,16 +772,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -795,10 +798,10 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -815,10 +818,10 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -843,13 +846,13 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -863,10 +866,10 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -874,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -883,14 +886,151 @@
         <v>31</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F12 D1:D12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F20 D1:D20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Page_Name</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G16" r:id="rId2" xr:uid="{AC2203A7-B801-4851-BB7A-92005B3E56EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -917,18 +1057,18 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -942,10 +1082,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -959,12 +1099,12 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>